<commit_message>
Update task pdf and billing
</commit_message>
<xml_diff>
--- a/CTF_Code.xlsx
+++ b/CTF_Code.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
   <si>
     <t xml:space="preserve">CTF Code</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Цена</t>
   </si>
   <si>
-    <t xml:space="preserve">SIGFPE</t>
+    <t xml:space="preserve">Crash me</t>
   </si>
   <si>
     <t xml:space="preserve">Binary Analysis</t>
@@ -49,103 +49,109 @@
     <t xml:space="preserve">Easy</t>
   </si>
   <si>
-    <t xml:space="preserve">Buffer Overflow</t>
+    <t xml:space="preserve">System health check</t>
   </si>
   <si>
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
-    <t xml:space="preserve">BO &amp; FS</t>
+    <t xml:space="preserve">You’re a Wizzard, Harry</t>
   </si>
   <si>
     <t xml:space="preserve">Hard</t>
   </si>
   <si>
-    <t xml:space="preserve">Use After Free</t>
+    <t xml:space="preserve">My anime list</t>
   </si>
   <si>
     <t xml:space="preserve">Real Life</t>
   </si>
   <si>
-    <t xml:space="preserve">GOT rewrite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Squirrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java</t>
+    <t xml:space="preserve">Arbalest shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Squirrel as a service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the license</t>
   </si>
   <si>
     <t xml:space="preserve">Reverse</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebApp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCAP USB</t>
+    <t xml:space="preserve">Guess the password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cryptowallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friendly VM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let’s GO for cookies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby keyboard</t>
   </si>
   <si>
     <t xml:space="preserve">Forensics</t>
   </si>
   <si>
-    <t xml:space="preserve">VM Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regex2Fat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stego-phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zip Random</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chrome history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base</t>
+    <t xml:space="preserve">Just log in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you hear it?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random xor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How about history?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based task</t>
   </si>
   <si>
     <t xml:space="preserve">Crypto</t>
   </si>
   <si>
-    <t xml:space="preserve">MD5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shamir Secret Sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ElGamal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EC DH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTP&amp;SSH logs</t>
+    <t xml:space="preserve">Hashes among us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please be careful with ASR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please don’t share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to play some gamel?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curve task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you true admin?</t>
   </si>
   <si>
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">Develop Base Brainfuck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 requests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICMP echo</t>
+    <t xml:space="preserve">Do you like black terminals with green text?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use your head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bash escape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too many files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just read the flag</t>
   </si>
   <si>
     <t xml:space="preserve">Итог: </t>
@@ -338,13 +344,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.47"/>
@@ -945,33 +951,73 @@
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="5" t="n">
         <f aca="false">_xlfn.SWITCH(F29,$L$3,$M$3,$L$4,$M$4,$L$5,$M$5,$L$6,$M$6)</f>
+        <v>2000</v>
+      </c>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="5" t="n">
+        <f aca="false">_xlfn.SWITCH(F30,$L$3,$M$3,$L$4,$M$4,$L$5,$M$5,$L$6,$M$6)</f>
         <v>3500</v>
       </c>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="6" t="n">
-        <f aca="false">SUM(H1:H29)</f>
-        <v>63500</v>
-      </c>
-      <c r="I30" s="6"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="5" t="n">
+        <f aca="false">_xlfn.SWITCH(F31,$L$3,$M$3,$L$4,$M$4,$L$5,$M$5,$L$6,$M$6)</f>
+        <v>5500</v>
+      </c>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="6" t="n">
+        <f aca="false">SUM(H3:H31)</f>
+        <v>71000</v>
+      </c>
+      <c r="I32" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="115">
+  <mergeCells count="123">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -1085,10 +1131,18 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:I29"/>
-    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
     <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="H32:I32"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:H29">
+  <conditionalFormatting sqref="H3:H31">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>